<commit_message>
Continuing to update dissertation
</commit_message>
<xml_diff>
--- a/DataSets/BotTableFull.xlsx
+++ b/DataSets/BotTableFull.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Dissertation_Artefact\DataSets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DCE54CD-205E-4478-9912-2BEB86D91481}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019677F3-EABD-4DA7-A11B-A736D332EE9F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12225" xr2:uid="{BC8A06F1-964C-48DB-A5B3-B6E40A83B283}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="280">
   <si>
     <t>Round/Game</t>
   </si>
@@ -862,6 +862,9 @@
   </si>
   <si>
     <t>20180503_175657</t>
+  </si>
+  <si>
+    <t>POSH Win</t>
   </si>
 </sst>
 </file>
@@ -1316,15 +1319,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1EE0FA3-6562-421F-A5CD-E86993C02C16}">
-  <dimension ref="A1:T82"/>
+  <dimension ref="A1:U82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:T82"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1385,8 +1388,11 @@
       <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U1" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1443,8 +1449,11 @@
       <c r="T2" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>28</v>
       </c>
@@ -1501,8 +1510,11 @@
       <c r="T3" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>32</v>
       </c>
@@ -1559,8 +1571,11 @@
       <c r="T4" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
@@ -1617,8 +1632,11 @@
       <c r="T5" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
@@ -1675,8 +1693,11 @@
       <c r="T6" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>44</v>
       </c>
@@ -1733,8 +1754,11 @@
       <c r="T7" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
@@ -1791,8 +1815,11 @@
       <c r="T8" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>52</v>
       </c>
@@ -1849,8 +1876,11 @@
       <c r="T9" s="7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>56</v>
       </c>
@@ -1907,8 +1937,11 @@
       <c r="T10" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>59</v>
       </c>
@@ -1965,8 +1998,11 @@
       <c r="T11" s="7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>62</v>
       </c>
@@ -2023,8 +2059,11 @@
       <c r="T12" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>65</v>
       </c>
@@ -2081,8 +2120,11 @@
       <c r="T13" s="7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>68</v>
       </c>
@@ -2139,8 +2181,11 @@
       <c r="T14" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>72</v>
       </c>
@@ -2197,8 +2242,11 @@
       <c r="T15" s="7" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>75</v>
       </c>
@@ -2255,8 +2303,11 @@
       <c r="T16" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>79</v>
       </c>
@@ -2313,8 +2364,11 @@
       <c r="T17" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>82</v>
       </c>
@@ -2371,8 +2425,11 @@
       <c r="T18" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>85</v>
       </c>
@@ -2429,8 +2486,11 @@
       <c r="T19" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>88</v>
       </c>
@@ -2487,8 +2547,11 @@
       <c r="T20" s="4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>91</v>
       </c>
@@ -2545,8 +2608,11 @@
       <c r="T21" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>94</v>
       </c>
@@ -2603,8 +2669,11 @@
       <c r="T22" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>97</v>
       </c>
@@ -2661,8 +2730,11 @@
       <c r="T23" s="7" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>100</v>
       </c>
@@ -2719,8 +2791,11 @@
       <c r="T24" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U24" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>103</v>
       </c>
@@ -2777,8 +2852,11 @@
       <c r="T25" s="7" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U25" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>106</v>
       </c>
@@ -2835,8 +2913,11 @@
       <c r="T26" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>109</v>
       </c>
@@ -2893,8 +2974,11 @@
       <c r="T27" s="7" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>112</v>
       </c>
@@ -2951,8 +3035,11 @@
       <c r="T28" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U28" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>115</v>
       </c>
@@ -3009,8 +3096,11 @@
       <c r="T29" s="7" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>118</v>
       </c>
@@ -3067,8 +3157,11 @@
       <c r="T30" s="4" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>121</v>
       </c>
@@ -3125,8 +3218,11 @@
       <c r="T31" s="7" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="32" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>124</v>
       </c>
@@ -3183,8 +3279,11 @@
       <c r="T32" s="4" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U32" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>127</v>
       </c>
@@ -3241,8 +3340,11 @@
       <c r="T33" s="7" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>130</v>
       </c>
@@ -3299,8 +3401,11 @@
       <c r="T34" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U34" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>133</v>
       </c>
@@ -3357,8 +3462,11 @@
       <c r="T35" s="7" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U35" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>136</v>
       </c>
@@ -3415,8 +3523,11 @@
       <c r="T36" s="4" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U36" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>139</v>
       </c>
@@ -3473,8 +3584,11 @@
       <c r="T37" s="7" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="38" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>142</v>
       </c>
@@ -3531,8 +3645,11 @@
       <c r="T38" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="39" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U38" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>145</v>
       </c>
@@ -3589,8 +3706,11 @@
       <c r="T39" s="7" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="40" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U39" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>148</v>
       </c>
@@ -3647,8 +3767,11 @@
       <c r="T40" s="4" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="41" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U40" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>151</v>
       </c>
@@ -3705,8 +3828,11 @@
       <c r="T41" s="7" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="42" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U41" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>154</v>
       </c>
@@ -3763,8 +3889,11 @@
       <c r="T42" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U42" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>157</v>
       </c>
@@ -3821,8 +3950,11 @@
       <c r="T43" s="7" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U43" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>160</v>
       </c>
@@ -3879,8 +4011,11 @@
       <c r="T44" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U44" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>163</v>
       </c>
@@ -3937,8 +4072,11 @@
       <c r="T45" s="7" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U45" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>166</v>
       </c>
@@ -3995,8 +4133,11 @@
       <c r="T46" s="4" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U46" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>170</v>
       </c>
@@ -4053,8 +4194,11 @@
       <c r="T47" s="7" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="48" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U47" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>173</v>
       </c>
@@ -4111,8 +4255,11 @@
       <c r="T48" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="49" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U48" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>176</v>
       </c>
@@ -4169,8 +4316,11 @@
       <c r="T49" s="7" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="50" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U49" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>179</v>
       </c>
@@ -4227,8 +4377,11 @@
       <c r="T50" s="4" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="51" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U50" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>182</v>
       </c>
@@ -4285,8 +4438,11 @@
       <c r="T51" s="7" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="52" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U51" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>185</v>
       </c>
@@ -4343,8 +4499,11 @@
       <c r="T52" s="4" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="53" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U52" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>188</v>
       </c>
@@ -4401,8 +4560,11 @@
       <c r="T53" s="7" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="54" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U53" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>191</v>
       </c>
@@ -4459,8 +4621,11 @@
       <c r="T54" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="55" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U54" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>194</v>
       </c>
@@ -4517,8 +4682,11 @@
       <c r="T55" s="7" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="56" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+      <c r="U55" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>197</v>
       </c>
@@ -4577,8 +4745,11 @@
       <c r="T56" s="4" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="57" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U56" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>201</v>
       </c>
@@ -4635,8 +4806,11 @@
       <c r="T57" s="7" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="58" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U57" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>204</v>
       </c>
@@ -4693,8 +4867,11 @@
       <c r="T58" s="4" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="59" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U58" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>207</v>
       </c>
@@ -4751,8 +4928,11 @@
       <c r="T59" s="7" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="60" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U59" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>210</v>
       </c>
@@ -4809,8 +4989,11 @@
       <c r="T60" s="4" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="61" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U60" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>213</v>
       </c>
@@ -4867,8 +5050,11 @@
       <c r="T61" s="7" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="62" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U61" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>216</v>
       </c>
@@ -4925,8 +5111,11 @@
       <c r="T62" s="4" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="63" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U62" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>219</v>
       </c>
@@ -4983,8 +5172,11 @@
       <c r="T63" s="7" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="64" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U63" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>222</v>
       </c>
@@ -5041,8 +5233,11 @@
       <c r="T64" s="4" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="65" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U64" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>225</v>
       </c>
@@ -5099,8 +5294,11 @@
       <c r="T65" s="7" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="66" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U65" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>228</v>
       </c>
@@ -5157,8 +5355,11 @@
       <c r="T66" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="67" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U66" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>231</v>
       </c>
@@ -5215,8 +5416,11 @@
       <c r="T67" s="7" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="68" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U67" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>234</v>
       </c>
@@ -5273,8 +5477,11 @@
       <c r="T68" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="69" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U68" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>237</v>
       </c>
@@ -5331,8 +5538,11 @@
       <c r="T69" s="7" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="70" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U69" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>240</v>
       </c>
@@ -5389,8 +5599,11 @@
       <c r="T70" s="4" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="71" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U70" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>243</v>
       </c>
@@ -5447,8 +5660,11 @@
       <c r="T71" s="7" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="72" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U71" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>246</v>
       </c>
@@ -5505,8 +5721,11 @@
       <c r="T72" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="73" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U72" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>249</v>
       </c>
@@ -5563,8 +5782,11 @@
       <c r="T73" s="7" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="74" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U73" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>252</v>
       </c>
@@ -5621,8 +5843,11 @@
       <c r="T74" s="4" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="75" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U74" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>255</v>
       </c>
@@ -5679,8 +5904,11 @@
       <c r="T75" s="4" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="76" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U75" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>258</v>
       </c>
@@ -5737,8 +5965,11 @@
       <c r="T76" s="7" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="77" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U76" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>261</v>
       </c>
@@ -5797,8 +6028,11 @@
       <c r="T77" s="4" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="78" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U77" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>264</v>
       </c>
@@ -5855,8 +6089,11 @@
       <c r="T78" s="7" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="79" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U78" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>267</v>
       </c>
@@ -5913,8 +6150,11 @@
       <c r="T79" s="4" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="80" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U79" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>270</v>
       </c>
@@ -5971,8 +6211,11 @@
       <c r="T80" s="7" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="81" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U80" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>273</v>
       </c>
@@ -6029,8 +6272,11 @@
       <c r="T81" s="4" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="82" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="U81" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>276</v>
       </c>
@@ -6086,6 +6332,9 @@
       </c>
       <c r="T82" s="7" t="s">
         <v>278</v>
+      </c>
+      <c r="U82" s="4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>